<commit_message>
updated RMD insight template
</commit_message>
<xml_diff>
--- a/RMD/input/insight.xlsx
+++ b/RMD/input/insight.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lidazhang/Downloads/DailyReport-master/RMD/input/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9E3C55-C974-9C4C-A513-223689AE0F78}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20720" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20715" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="工作表 1 - test" sheetId="1" r:id="rId1"/>
@@ -20,29 +14,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>content</t>
   </si>
   <si>
-    <t> 截止北京时间4月3日早5:00，全球累计确诊病例超过100万人(1,075,777)，累计死亡52,772例。由图1所示，确诊病例全球分布广泛，主要集中在美国、亚洲、欧洲以及中东地区，在南美、澳大利亚以及非洲部分地区也有散在分布。由表1所示，累计确诊人数前三位的国家仍然为美国，意大利和西班牙。德国首次超过中国成为第四位。粗发病率最高的国家是西班牙和瑞士，均在200/10万人以上。此外，澳大利亚、加拿大累计确诊数均已超过1万人。</t>
+    <t>section</t>
   </si>
   <si>
-    <t>    从表2和图2来看，美国新增病例数居全球首位，连续三天每日新增病例数稳定在约两万五千人。德国新增病例数近三日有小幅升高的趋势。法国新增病例数于3月31日达到近期峰值（7,657），近两日每日减少约2500人，疫情有趋稳的迹象。加拿大新增病例数进入前十位。此外，南美洲的巴西近三日新增病例数达到千人以上，南亚的印度新增病例数由3月31号之前的200人以下升高至500人以上。
-    从累计死亡病例数（表3和图3）来看，多数国家新增死亡病例数及病死率稳定。法国新增死亡病例数较昨日（+511人）升高幅度明显增加，病死率由7%升高到9%。美国和西班牙新增死亡数较昨日升高约300人，但病死率升高幅度不大（+0.3%）。</t>
+    <t>page2</t>
   </si>
   <si>
-    <t xml:space="preserve"> 截至北京时间4月3日早5:00， 美国累计确诊病例数已达到238,820例，共 5,758例死亡病例。从州疫情分布图（图4，图5）来看，确诊病例主要集中于沿海地区，对比前几日数据可见逐步向中部蔓延，有全国爆发趋势。
- 纽约州(NY)粗发病率达到475/10万人，累计确诊数占全美39%，较昨日有所降低（41%），日新增确诊数较昨日小幅提高，但占全美比例较昨日（44%）有所下降，提示其他州的疫情有进一步恶化的趋势。密歇根州、加利福尼亚州累计确诊人数均已超过1万人。路易斯安纳州（LA）新增确诊病例数进一步上升，由昨日的1187人升至2697人。密歇根州（MI）、宾夕法尼亚州（PA）以及佛罗里达州（FL）新增确诊病例数均超过一千人，提示疫情在美国迅速蔓延趋势。</t>
+    <t>page3</t>
   </si>
   <si>
-    <t xml:space="preserve"> 从表6来看，全美累计阳性率前四位阳性率均为接近40%及以上，提示有大量轻症及无症状感染者未被检出，感染人数远超报告数字，疫情严峻。全美共检测126.7万人，累计检测人数最多的三个州是纽约州（23.9万人）、佛罗里达州（7.7万人）及华盛顿州（7.5万人），其中佛罗里达州及华盛顿州阳性率均在10%以下，提示疫情控较好。从表7全国累计死亡人数来看，各州死亡人数继续增高，病死率较昨日较为稳定。其中纽约州的累计死亡病例最多，病死率为2.6%，略高于全国平均病死率。华盛顿州、密歇根州及路易斯安娜州的病死率也均明显高于全国平均。</t>
+    <t>page4</t>
+  </si>
+  <si>
+    <t>page5</t>
+  </si>
+  <si>
+    <t>  截止北京时间4月3日早5:00，全球累计确诊病例超过100万人(1,075,777)，累计死亡52,772例。由图1所示，确诊病例全球分布广泛，主要集中在美国、亚洲、欧洲以及中东地区，在南美、澳大利亚以及非洲部分地区也有散在分布。由表1所示，累计确诊人数前三位的国家仍然为美国，意大利和西班牙。德国首次超过中国成为第四位。粗发病率最高的国家是西班牙和瑞士，均在200/10万人以上。此外，澳大利亚、加拿大累计确诊数均已超过1万人。
+  XXXXXXX。</t>
+  </si>
+  <si>
+    <t>  从表2和图2来看，美国新增病例数居全球首位，连续三天每日新增病例数稳定在约两万五千人。德国新增病例数近三日有小幅升高的趋势。法国新增病例数于3月31日达到近期峰值（7,657），近两日每日减少约2500人，疫情有趋稳的迹象。加拿大新增病例数进入前十位。此外，南美洲的巴西近三日新增病例数达到千人以上，南亚的印度新增病例数由3月31号之前的200人以下升高至500人以上。
+  从累计死亡病例数（表3和图3）来看，多数国家新增死亡病例数及病死率稳定。法国新增死亡病例数较昨日（+511人）升高幅度明显增加，病死率由7%升高到9%。美国和西班牙新增死亡数较昨日升高约300人，但病死率升高幅度不大（+0.3%）。</t>
+  </si>
+  <si>
+    <t>  截至北京时间4月3日早5:00， 美国累计确诊病例数已达到238,820例，共 5,758例死亡病例。从州疫情分布图（图4，图5）来看，确诊病例主要集中于沿海地区，对比前几日数据可见逐步向中部蔓延，有全国爆发趋势。
+  纽约州(NY)粗发病率达到475/10万人，累计确诊数占全美39%，较昨日有所降低（41%），日新增确诊数较昨日小幅提高，但占全美比例较昨日（44%）有所下降，提示其他州的疫情有进一步恶化的趋势。密歇根州、加利福尼亚州累计确诊人数均已超过1万人。路易斯安纳州（LA）新增确诊病例数进一步上升，由昨日的1187人升至2697人。密歇根州（MI）、宾夕法尼亚州（PA）以及佛罗里达州（FL）新增确诊病例数均超过一千人，提示疫情在美国迅速蔓延趋势。</t>
+  </si>
+  <si>
+    <t>  从表6来看，全美累计阳性率前四位阳性率均为接近40%及以上，提示有大量轻症及无症状感染者未被检出，感染人数远超报告数字，疫情严峻。全美共检测126.7万人，累计检测人数最多的三个州是纽约州（23.9万人）、佛罗里达州（7.7万人）及华盛顿州（7.5万人），其中佛罗里达州及华盛顿州阳性率均在10%以下，提示疫情控较好。从表7全国累计死亡人数来看，各州死亡人数继续增高，病死率较昨日较为稳定。其中纽约州的累计死亡病例最多，病死率为2.6%，略高于全国平均病死率。华盛顿州、密歇根州及路易斯安娜州的病死率也均明显高于全国平均。
+  XXXXXXX.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -56,10 +67,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="13.95"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="SimSun"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -76,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,36 +96,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -129,19 +119,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1303,62 +1293,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="147.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.33203125" style="1"/>
+    <col min="1" max="1" width="8.28515625" style="1"/>
+    <col min="2" max="2" width="147.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="20" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="20" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="20" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.75" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.75" customHeight="1">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:2" ht="14.85" customHeight="1">
+      <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:1" ht="14.75" customHeight="1">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:2" ht="14.85" customHeight="1">
+      <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:1" ht="14.75" customHeight="1">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:2" ht="14.85" customHeight="1">
+      <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:1" ht="14.75" customHeight="1">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:2" ht="14.85" customHeight="1">
+      <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:1" ht="14.75" customHeight="1">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:2" ht="14.85" customHeight="1">
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>